<commit_message>
GUI improved with customtkinter
</commit_message>
<xml_diff>
--- a/Day 1.xlsx
+++ b/Day 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSBDA-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSBDA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB689190-0A56-42D2-BB50-53C39BB8DAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02E3DBF-7DCA-4228-B50F-B558487AEAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Manish</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +450,7 @@
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -490,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -513,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -536,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -559,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -582,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -605,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -616,7 +622,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -628,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -639,7 +645,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -651,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -674,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -685,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -697,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -720,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -731,7 +737,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -741,6 +747,32 @@
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>